<commit_message>
fixed sorting of plot selector
fixed sorting, the ascending/descending doesn't seem to matter though.
</commit_message>
<xml_diff>
--- a/resources/app_data/element_info.xlsx
+++ b/resources/app_data/element_info.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a1904121/LaserMapExplorer/LaserMapExplorerPyQT/LaserMapExplorer/resources/app_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhasterok/Documents/LaserMapExplorer/resources/app_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5852C4B-C8F4-A349-97FA-51874A08A345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5538E66-2802-5E4B-BF83-901B976A421E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6300" yWindow="2600" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,19 @@
     <sheet name="element_info" sheetId="1" r:id="rId1"/>
     <sheet name="isotope_info" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1500,10 +1512,10 @@
   <dimension ref="A1:U85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E72" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D1" sqref="D1:D1048576"/>
+      <selection pane="bottomRight" activeCell="V2" sqref="V2:V85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1617,7 +1629,7 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="T2">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="U2" t="s">
         <v>192</v>
@@ -1661,7 +1673,7 @@
         <v>0.53500000000000003</v>
       </c>
       <c r="T3">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="U3" t="s">
         <v>198</v>
@@ -1749,7 +1761,7 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="T5">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="U5" t="s">
         <v>192</v>
@@ -1799,7 +1811,7 @@
         <v>1.37</v>
       </c>
       <c r="T6">
-        <v>69</v>
+        <v>2</v>
       </c>
       <c r="U6" t="s">
         <v>193</v>
@@ -1840,7 +1852,7 @@
         <v>0.27</v>
       </c>
       <c r="T7">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="U7" t="s">
         <v>198</v>
@@ -1887,7 +1899,7 @@
         <v>1.2E-4</v>
       </c>
       <c r="T8">
-        <v>3</v>
+        <v>68</v>
       </c>
       <c r="U8" t="s">
         <v>196</v>
@@ -1931,7 +1943,7 @@
         <v>0.45</v>
       </c>
       <c r="T9">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="U9" t="s">
         <v>198</v>
@@ -1984,7 +1996,7 @@
         <v>0.76</v>
       </c>
       <c r="T10">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="U10" t="s">
         <v>192</v>
@@ -2104,7 +2116,7 @@
         <v>1</v>
       </c>
       <c r="T13">
-        <v>8</v>
+        <v>63</v>
       </c>
       <c r="U13" t="s">
         <v>196</v>
@@ -2148,7 +2160,7 @@
         <v>0.95</v>
       </c>
       <c r="T14">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="U14" t="s">
         <v>192</v>
@@ -2204,7 +2216,7 @@
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="T15">
-        <v>12</v>
+        <v>59</v>
       </c>
       <c r="U15" t="s">
         <v>195</v>
@@ -2295,7 +2307,7 @@
         <v>0.54500000000000004</v>
       </c>
       <c r="T17">
-        <v>65</v>
+        <v>6</v>
       </c>
       <c r="U17" t="s">
         <v>193</v>
@@ -2348,7 +2360,7 @@
         <v>0.61499999999999999</v>
       </c>
       <c r="T18">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="U18" t="s">
         <v>198</v>
@@ -2392,7 +2404,7 @@
         <v>1.67</v>
       </c>
       <c r="T19">
-        <v>1</v>
+        <v>70</v>
       </c>
       <c r="U19" t="s">
         <v>196</v>
@@ -2445,7 +2457,7 @@
         <v>0.73</v>
       </c>
       <c r="T20">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="U20" t="s">
         <v>192</v>
@@ -2501,7 +2513,7 @@
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="T21">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="U21" t="s">
         <v>195</v>
@@ -2548,7 +2560,7 @@
         <v>9.7000000000000003E-2</v>
       </c>
       <c r="T22">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="U22" t="s">
         <v>195</v>
@@ -2604,7 +2616,7 @@
         <v>0.05</v>
       </c>
       <c r="T23">
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="U23" t="s">
         <v>195</v>
@@ -2698,7 +2710,7 @@
         <v>0.64500000000000002</v>
       </c>
       <c r="T25">
-        <v>66</v>
+        <v>5</v>
       </c>
       <c r="U25" t="s">
         <v>193</v>
@@ -2742,7 +2754,7 @@
         <v>0.62</v>
       </c>
       <c r="T26">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="U26" t="s">
         <v>198</v>
@@ -2789,7 +2801,7 @@
         <v>5.6000000000000001E-2</v>
       </c>
       <c r="T27">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="U27" t="s">
         <v>195</v>
@@ -2842,7 +2854,7 @@
         <v>0.53</v>
       </c>
       <c r="T28">
-        <v>67</v>
+        <v>4</v>
       </c>
       <c r="U28" t="s">
         <v>193</v>
@@ -2965,7 +2977,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="T31">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="U31" t="s">
         <v>194</v>
@@ -3009,7 +3021,7 @@
         <v>1.19</v>
       </c>
       <c r="T32">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="U32" t="s">
         <v>192</v>
@@ -3056,7 +3068,7 @@
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="T33">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="U33" t="s">
         <v>195</v>
@@ -3141,7 +3153,7 @@
         <v>0.8</v>
       </c>
       <c r="T35">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="U35" t="s">
         <v>192</v>
@@ -3185,7 +3197,7 @@
         <v>0.625</v>
       </c>
       <c r="T36">
-        <v>61</v>
+        <v>10</v>
       </c>
       <c r="U36" t="s">
         <v>193</v>
@@ -3229,7 +3241,7 @@
         <v>1.38</v>
       </c>
       <c r="T37">
-        <v>4</v>
+        <v>67</v>
       </c>
       <c r="U37" t="s">
         <v>196</v>
@@ -3314,7 +3326,7 @@
         <v>0.01</v>
       </c>
       <c r="T39">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="U39" t="s">
         <v>195</v>
@@ -3355,7 +3367,7 @@
         <v>0.76</v>
       </c>
       <c r="T40">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="U40" t="s">
         <v>198</v>
@@ -3402,7 +3414,7 @@
         <v>0.12</v>
       </c>
       <c r="T41">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="U41" t="s">
         <v>195</v>
@@ -3443,7 +3455,7 @@
         <v>0.72</v>
       </c>
       <c r="T42">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="U42" t="s">
         <v>198</v>
@@ -3505,7 +3517,7 @@
         <v>0.53</v>
       </c>
       <c r="T43">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="U43" t="s">
         <v>198</v>
@@ -3558,7 +3570,7 @@
         <v>0.59</v>
       </c>
       <c r="T44">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="U44" t="s">
         <v>192</v>
@@ -3649,7 +3661,7 @@
         <v>1.02</v>
       </c>
       <c r="T46">
-        <v>7</v>
+        <v>64</v>
       </c>
       <c r="U46" t="s">
         <v>196</v>
@@ -3705,7 +3717,7 @@
         <v>3.3999999999999998E-3</v>
       </c>
       <c r="T47">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="U47" t="s">
         <v>194</v>
@@ -3752,7 +3764,7 @@
         <v>3.1E-2</v>
       </c>
       <c r="T48">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="U48" t="s">
         <v>195</v>
@@ -3843,7 +3855,7 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="T50">
-        <v>64</v>
+        <v>7</v>
       </c>
       <c r="U50" t="s">
         <v>193</v>
@@ -3925,7 +3937,7 @@
         <v>0.63</v>
       </c>
       <c r="T52">
-        <v>62</v>
+        <v>9</v>
       </c>
       <c r="U52" t="s">
         <v>193</v>
@@ -3969,7 +3981,7 @@
         <v>0.38</v>
       </c>
       <c r="T53">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="U53" t="s">
         <v>200</v>
@@ -4051,7 +4063,7 @@
         <v>1.4E-2</v>
       </c>
       <c r="T55">
-        <v>6</v>
+        <v>65</v>
       </c>
       <c r="U55" t="s">
         <v>196</v>
@@ -4092,7 +4104,7 @@
         <v>1.37</v>
       </c>
       <c r="T56">
-        <v>68</v>
+        <v>3</v>
       </c>
       <c r="U56" t="s">
         <v>193</v>
@@ -4139,7 +4151,7 @@
         <v>2.7E-2</v>
       </c>
       <c r="T57">
-        <v>13</v>
+        <v>58</v>
       </c>
       <c r="U57" t="s">
         <v>195</v>
@@ -4189,7 +4201,7 @@
         <v>0.8</v>
       </c>
       <c r="T58">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="U58" t="s">
         <v>193</v>
@@ -4236,7 +4248,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="T59">
-        <v>2</v>
+        <v>69</v>
       </c>
       <c r="U59" t="s">
         <v>196</v>
@@ -4280,7 +4292,7 @@
         <v>0.63</v>
       </c>
       <c r="T60">
-        <v>58</v>
+        <v>13</v>
       </c>
       <c r="U60" t="s">
         <v>193</v>
@@ -4324,7 +4336,7 @@
         <v>0.66500000000000004</v>
       </c>
       <c r="T61">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="U61" t="s">
         <v>193</v>
@@ -4377,7 +4389,7 @@
         <v>0.62</v>
       </c>
       <c r="T62">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="U62" t="s">
         <v>193</v>
@@ -4427,7 +4439,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="T63">
-        <v>57</v>
+        <v>14</v>
       </c>
       <c r="U63" t="s">
         <v>192</v>
@@ -4471,7 +4483,7 @@
         <v>0.6</v>
       </c>
       <c r="T64">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="U64" t="s">
         <v>192</v>
@@ -4515,7 +4527,7 @@
         <v>0.745</v>
       </c>
       <c r="T65">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="U65" t="s">
         <v>198</v>
@@ -4559,7 +4571,7 @@
         <v>1.98</v>
       </c>
       <c r="T66">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="U66" t="s">
         <v>192</v>
@@ -4600,7 +4612,7 @@
         <v>0.4</v>
       </c>
       <c r="T67">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="U67" t="s">
         <v>198</v>
@@ -4647,7 +4659,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="T68">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="U68" t="s">
         <v>195</v>
@@ -4691,7 +4703,7 @@
         <v>0.69</v>
       </c>
       <c r="T69">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="U69" t="s">
         <v>192</v>
@@ -4738,7 +4750,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="T70">
-        <v>5</v>
+        <v>66</v>
       </c>
       <c r="U70" t="s">
         <v>196</v>
@@ -4785,7 +4797,7 @@
         <v>3.3999999999999998E-3</v>
       </c>
       <c r="T71">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="U71" t="s">
         <v>194</v>
@@ -4841,7 +4853,7 @@
         <v>6.8000000000000005E-2</v>
       </c>
       <c r="T72">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="U72" t="s">
         <v>195</v>
@@ -4894,7 +4906,7 @@
         <v>2.21</v>
       </c>
       <c r="T73">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="U73" t="s">
         <v>192</v>
@@ -4941,7 +4953,7 @@
         <v>1E-3</v>
       </c>
       <c r="T74">
-        <v>9</v>
+        <v>62</v>
       </c>
       <c r="U74" t="s">
         <v>196</v>
@@ -5006,7 +5018,7 @@
         <v>5.8000000000000003E-2</v>
       </c>
       <c r="T75">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="U75" t="s">
         <v>198</v>
@@ -5056,7 +5068,7 @@
         <v>1.5</v>
       </c>
       <c r="T76">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="U76" t="s">
         <v>192</v>
@@ -5109,7 +5121,7 @@
         <v>1.03</v>
       </c>
       <c r="T77">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="U77" t="s">
         <v>195</v>
@@ -5165,7 +5177,7 @@
         <v>1.1000000000000001E-3</v>
       </c>
       <c r="T78">
-        <v>10</v>
+        <v>61</v>
       </c>
       <c r="U78" t="s">
         <v>196</v>
@@ -5227,7 +5239,7 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="T79">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="U79" t="s">
         <v>198</v>
@@ -5271,7 +5283,7 @@
         <v>0.6</v>
       </c>
       <c r="T80">
-        <v>70</v>
+        <v>1</v>
       </c>
       <c r="U80" t="s">
         <v>193</v>
@@ -5356,7 +5368,7 @@
         <v>8.7999999999999995E-2</v>
       </c>
       <c r="T82">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="U82" t="s">
         <v>195</v>
@@ -5412,7 +5424,7 @@
         <v>0.115</v>
       </c>
       <c r="T83">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="U83" t="s">
         <v>195</v>
@@ -5456,7 +5468,7 @@
         <v>0.74</v>
       </c>
       <c r="T84">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="U84" t="s">
         <v>192</v>
@@ -5503,7 +5515,7 @@
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="T85">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="U85" t="s">
         <v>194</v>

</xml_diff>